<commit_message>
Revent data cleaning and new diagram
Former-commit-id: 978c1c0c2623677581e1b1ddcb6db5527ad6059c
</commit_message>
<xml_diff>
--- a/Swift_Experiments/strategy_1/analysis/strategy_1_analysis_cleaned.xlsx
+++ b/Swift_Experiments/strategy_1/analysis/strategy_1_analysis_cleaned.xlsx
@@ -24,11 +24,14 @@
   <definedNames>
     <definedName name="Te_Executing_task_stampede" localSheetId="2">Te_stampede!$B$4:$E$7</definedName>
     <definedName name="Te_Executing_task_stampede_gordon" localSheetId="5">Te_stampede_gordon!$B$4:$E$11</definedName>
+    <definedName name="Te_Executing_task_stampede_gordon_1" localSheetId="5">Te_stampede_gordon!$B$4:$E$11</definedName>
     <definedName name="TTC_Time_to_completion_stampede" localSheetId="0">TTC_stampede!$B$4:$E$7</definedName>
     <definedName name="TTC_Time_to_completion_stampede_gordon" localSheetId="3">TTC_stampede_gordon!$B$4:$E$11</definedName>
     <definedName name="TTC_Time_to_completion_stampede_gordon_1" localSheetId="3">TTC_stampede_gordon!$B$16:$E$23</definedName>
+    <definedName name="TTC_Time_to_completion_stampede_gordon_2" localSheetId="3">TTC_stampede_gordon!$B$4:$E$11</definedName>
     <definedName name="Tw_Submitting_task_stampede" localSheetId="1">Tw_stampede!$B$4:$E$7</definedName>
     <definedName name="Tw_Submitting_task_stampede_gordon" localSheetId="4">Tw_stampede_gordon!$B$4:$E$11</definedName>
+    <definedName name="Tw_Submitting_task_stampede_gordon_1" localSheetId="4">Tw_stampede_gordon!$B$4:$E$11</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -64,7 +67,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="TTC-Time_to_completion-stampede" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="Te-Executing_task-stampede_gordon1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/Te-Executing_task-stampede_gordon.csv" tab="0" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="TTC-Time_to_completion-stampede" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede/TTC-Time_to_completion-stampede.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -74,7 +87,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="TTC-Time_to_completion-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="TTC-Time_to_completion-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/TTC-Time_to_completion-stampede_gordon.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -84,7 +97,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="TTC-Time_to_completion-stampede_gordon1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="TTC-Time_to_completion-stampede_gordon1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/TTC-Time_to_completion-stampede_gordon.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -94,7 +107,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="Tw-Submitting_task-stampede" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="TTC-Time_to_completion-stampede_gordon2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/TTC-Time_to_completion-stampede_gordon.csv" tab="0" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="Tw-Submitting_task-stampede" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede/Tw-Submitting_task-stampede.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -104,7 +127,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="Tw-Submitting_task-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="Tw-Submitting_task-stampede_gordon" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/Tw-Submitting_task-stampede_gordon.csv" tab="0" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" name="Tw-Submitting_task-stampede_gordon1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" firstRow="2" sourceFile="/Users/mturilli/Projects/RADICAL/github/experiments/AIMES-Swift/Swift_Experiments/strategy_1/analysis/stampede_gordon/Tw-Submitting_task-stampede_gordon.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -308,7 +341,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -321,16 +354,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Time to Completion (TTC) - Swift+Coaster</a:t>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Time to Completion (TTC) - Swift</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t> on </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
               <a:t>Stampede and Gordon</a:t>
             </a:r>
           </a:p>
@@ -350,7 +382,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -376,10 +408,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>TTC</c:v>
+            <c:v>TTCmeasured</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -414,16 +446,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3045.356652972272</c:v>
+                    <c:v>2572.521799386541</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2375.572890718963</c:v>
+                    <c:v>1968.50174712929</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3634.250914963257</c:v>
+                    <c:v>2996.508383312232</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10871.77024484303</c:v>
+                    <c:v>9368.497545766083</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -435,16 +467,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>3045.356652972272</c:v>
+                    <c:v>2572.521799386541</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2375.572890718963</c:v>
+                    <c:v>1968.50174712929</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3634.250914963257</c:v>
+                    <c:v>2996.508383312232</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>10871.77024484303</c:v>
+                    <c:v>9368.497545766083</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -488,16 +520,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11106.45400538219</c:v>
+                  <c:v>9001.463688459622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8476.67085824398</c:v>
+                  <c:v>7294.213835455774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11960.97268297247</c:v>
+                  <c:v>10042.610012873</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47912.11183556561</c:v>
+                  <c:v>39437.87776492022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,10 +540,10 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Ideal</c:v>
+            <c:v>TTCideal</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -584,7 +616,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -597,7 +629,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Number of Tasks</a:t>
                 </a:r>
               </a:p>
@@ -617,7 +649,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -655,7 +687,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -706,7 +738,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -719,14 +751,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t> (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="2000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -744,7 +776,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -776,7 +808,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -804,6 +836,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -813,12 +877,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -862,7 +921,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -875,41 +934,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
-              <a:t>Waiting Time (Tw) - Swift+Coaster</a:t>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Waiting Time (Tw) - Swift</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t> on </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
               <a:t>Stampede and Gordon</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Includes: setup</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>, queueing , and bootstrapping times. </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Queuing time accounts for the majority of the timing and of the variation.  </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -927,7 +963,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -956,9 +992,9 @@
             <c:v>Tw</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="12700" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -969,11 +1005,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -991,16 +1027,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>6194.515450514807</c:v>
+                    <c:v>4262.36272898989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5451.109908006503</c:v>
+                    <c:v>3216.387585197761</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8186.158382446555</c:v>
+                    <c:v>4706.366143510905</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>15747.10732430986</c:v>
+                    <c:v>13493.07197892946</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1012,16 +1048,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>6194.515450514807</c:v>
+                    <c:v>4262.36272898989</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5451.109908006503</c:v>
+                    <c:v>3216.387585197761</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8186.158382446555</c:v>
+                    <c:v>4706.366143510905</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>15747.10732430986</c:v>
+                    <c:v>13493.07197892946</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1065,16 +1101,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16736.0</c:v>
+                  <c:v>8392.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11440.75</c:v>
+                  <c:v>6557.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15777.75</c:v>
+                  <c:v>8573.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60593.5</c:v>
+                  <c:v>30558.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,7 +1144,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1121,7 +1157,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Number of Tasks</a:t>
                 </a:r>
               </a:p>
@@ -1141,7 +1177,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1179,7 +1215,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1230,7 +1266,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1243,14 +1279,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000"/>
                   <a:t>Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
                   <a:t> (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="2000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1268,7 +1304,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1300,7 +1336,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1327,6 +1363,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1336,12 +1404,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1514,16 +1577,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>71.9981191883973</c:v>
+                    <c:v>138.1061638740285</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>225.7559523024808</c:v>
+                    <c:v>162.1808679486314</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>633.4588910629218</c:v>
+                    <c:v>471.2409505572949</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3444.390620995244</c:v>
+                    <c:v>2746.114144178487</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1535,16 +1598,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>71.9981191883973</c:v>
+                    <c:v>138.1061638740285</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>225.7559523024808</c:v>
+                    <c:v>162.1808679486314</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>633.4588910629218</c:v>
+                    <c:v>471.2409505572949</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3444.390620995244</c:v>
+                    <c:v>2746.114144178487</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1588,16 +1651,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1759.75</c:v>
+                  <c:v>1408.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1605.5</c:v>
+                  <c:v>1395.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3188.0</c:v>
+                  <c:v>2333.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17805.5</c:v>
+                  <c:v>12470.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7212,11 +7275,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-stampede" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-stampede" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7224,19 +7291,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-stampede_gordon" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-stampede_gordon_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tw-Submitting_task-stampede_gordon" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8000,8 +8075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8031,19 +8106,19 @@
       </c>
       <c r="B2" s="5">
         <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
-        <v>11106.454005382189</v>
+        <v>9001.4636884596221</v>
       </c>
       <c r="C2" s="6">
         <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
-        <v>8476.6708582439805</v>
+        <v>7294.2138354557746</v>
       </c>
       <c r="D2" s="6">
         <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
-        <v>11960.97268297247</v>
+        <v>10042.610012873003</v>
       </c>
       <c r="E2" s="6">
         <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
-        <v>47912.111835565607</v>
+        <v>39437.877764920217</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -8052,19 +8127,19 @@
       </c>
       <c r="B3" s="2">
         <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
-        <v>3045.3566529722721</v>
+        <v>2572.5217993865408</v>
       </c>
       <c r="C3" s="2">
         <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
-        <v>2375.5728907189628</v>
+        <v>1968.5017471292904</v>
       </c>
       <c r="D3" s="2">
         <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
-        <v>3634.2509149632574</v>
+        <v>2996.5083833122321</v>
       </c>
       <c r="E3" s="2">
         <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
-        <v>10871.770244843028</v>
+        <v>9368.4975457660839</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -8072,48 +8147,48 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1650</v>
+        <v>1119</v>
       </c>
       <c r="C4">
-        <v>1027</v>
+        <v>8373</v>
       </c>
       <c r="D4">
-        <v>2123</v>
+        <v>7972</v>
       </c>
       <c r="E4">
-        <v>41107</v>
+        <v>15348</v>
       </c>
       <c r="G4">
         <f>Tw_stampede_gordon!B4+((B1*1200)/L4)</f>
-        <v>1649</v>
+        <v>1117</v>
       </c>
       <c r="H4">
         <f>Tw_stampede_gordon!C4+((C1*1200)/M4)</f>
-        <v>1026</v>
+        <v>8372</v>
       </c>
       <c r="I4">
         <f>Tw_stampede_gordon!D4+((D1*1200)/N4)</f>
-        <v>2122</v>
+        <v>7970</v>
       </c>
       <c r="J4">
         <f>Tw_stampede_gordon!E4+((E1*1200)/O4)</f>
-        <v>41106</v>
+        <v>15347</v>
       </c>
       <c r="L4">
         <f>(B1*1200)/Te_stampede_gordon!B4</f>
-        <v>6.2176165803108807</v>
+        <v>9.0737240075614363</v>
       </c>
       <c r="M4">
         <f>(C1*1200)/Te_stampede_gordon!C4</f>
-        <v>41.245972073039745</v>
+        <v>21.309655937846838</v>
       </c>
       <c r="N4">
         <f>(D1*1200)/Te_stampede_gordon!D4</f>
-        <v>150.29354207436398</v>
+        <v>116.67299658184581</v>
       </c>
       <c r="O4">
         <f>(E1*1200)/Te_stampede_gordon!E4</f>
-        <v>243.95473496128648</v>
+        <v>183.81451009723261</v>
       </c>
       <c r="Q4">
         <v>1200</v>
@@ -8133,48 +8208,48 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>29871</v>
+        <v>1224</v>
       </c>
       <c r="C5">
-        <v>28128</v>
+        <v>1041</v>
       </c>
       <c r="D5">
-        <v>15061</v>
+        <v>1158</v>
       </c>
       <c r="E5">
-        <v>74328</v>
+        <v>5619</v>
       </c>
       <c r="G5">
         <f>Tw_stampede_gordon!B5+((B2*1200)/L5)</f>
-        <v>29870</v>
+        <v>1223</v>
       </c>
       <c r="H5">
         <f>Tw_stampede_gordon!C5+((C2*1200)/M5)</f>
-        <v>28127</v>
+        <v>1039</v>
       </c>
       <c r="I5">
         <f>Tw_stampede_gordon!D5+((D2*1200)/N5)</f>
-        <v>15060</v>
+        <v>1157</v>
       </c>
       <c r="J5">
         <f>Tw_stampede_gordon!E5+((E2*1200)/O5)</f>
-        <v>74327</v>
+        <v>5618.0000000000009</v>
       </c>
       <c r="L5">
         <f>(B2*1200)/Te_stampede_gordon!B5</f>
-        <v>7255.1686480449798</v>
+        <v>9216.5157219723078</v>
       </c>
       <c r="M5">
         <f>(C2*1200)/Te_stampede_gordon!C5</f>
-        <v>5647.9761409732237</v>
+        <v>8886.3518807583041</v>
       </c>
       <c r="N5">
         <f>(D2*1200)/Te_stampede_gordon!D5</f>
-        <v>3809.2269690995126</v>
+        <v>10906.001823934483</v>
       </c>
       <c r="O5">
         <f>(E2*1200)/Te_stampede_gordon!E5</f>
-        <v>2312.1746240922835</v>
+        <v>8478.2252450562974</v>
       </c>
       <c r="Q5">
         <v>1200</v>
@@ -8194,48 +8269,48 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>25824</v>
+        <v>1034</v>
       </c>
       <c r="C6">
-        <v>11645</v>
+        <v>1020</v>
       </c>
       <c r="D6">
-        <v>15195</v>
+        <v>1127</v>
       </c>
       <c r="E6">
-        <v>127092</v>
+        <v>4869</v>
       </c>
       <c r="G6">
         <f>Tw_stampede_gordon!B6+((B3*1200)/L6)</f>
-        <v>25823</v>
+        <v>1033</v>
       </c>
       <c r="H6">
         <f>Tw_stampede_gordon!C6+((C3*1200)/M6)</f>
-        <v>11644</v>
+        <v>1019</v>
       </c>
       <c r="I6">
         <f>Tw_stampede_gordon!D6+((D3*1200)/N6)</f>
-        <v>15194</v>
+        <v>1126</v>
       </c>
       <c r="J6">
         <f>Tw_stampede_gordon!E6+((E3*1200)/O6)</f>
-        <v>127091</v>
+        <v>4867</v>
       </c>
       <c r="L6">
         <f>(B3*1200)/Te_stampede_gordon!B6</f>
-        <v>1990.4291849491974</v>
+        <v>3143.6111601464854</v>
       </c>
       <c r="M6">
         <f>(C3*1200)/Te_stampede_gordon!C6</f>
-        <v>1509.8980237620526</v>
+        <v>2403.0540148068649</v>
       </c>
       <c r="N6">
         <f>(D3*1200)/Te_stampede_gordon!D6</f>
-        <v>1944.3161381881002</v>
+        <v>3370.0188003511512</v>
       </c>
       <c r="O6">
         <f>(E3*1200)/Te_stampede_gordon!E6</f>
-        <v>588.37885237954424</v>
+        <v>2329.0236285310339</v>
       </c>
       <c r="Q6">
         <v>1200</v>
@@ -8255,48 +8330,48 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16642</v>
+        <v>1054</v>
       </c>
       <c r="C7">
-        <v>11392</v>
+        <v>1006</v>
       </c>
       <c r="D7">
-        <v>43488</v>
+        <v>1138</v>
       </c>
       <c r="E7">
-        <v>71073</v>
+        <v>4802</v>
       </c>
       <c r="G7">
         <f>Tw_stampede_gordon!B7+((B4*1200)/L7)</f>
-        <v>16641</v>
+        <v>1053</v>
       </c>
       <c r="H7">
         <f>Tw_stampede_gordon!C7+((C4*1200)/M7)</f>
-        <v>11388</v>
+        <v>1005</v>
       </c>
       <c r="I7">
         <f>Tw_stampede_gordon!D7+((D4*1200)/N7)</f>
-        <v>43487</v>
+        <v>1137</v>
       </c>
       <c r="J7">
         <f>Tw_stampede_gordon!E7+((E4*1200)/O7)</f>
-        <v>71072</v>
+        <v>4800</v>
       </c>
       <c r="L7">
         <f>(B4*1200)/Te_stampede_gordon!B7</f>
-        <v>1086.7178924259056</v>
+        <v>1317.7625122669283</v>
       </c>
       <c r="M7">
         <f>(C4*1200)/Te_stampede_gordon!C7</f>
-        <v>683.90677025527191</v>
+        <v>10358.350515463917</v>
       </c>
       <c r="N7">
         <f>(D4*1200)/Te_stampede_gordon!D7</f>
-        <v>542.38875878220142</v>
+        <v>8618.3783783783783</v>
       </c>
       <c r="O7">
         <f>(E4*1200)/Te_stampede_gordon!E7</f>
-        <v>3496.2364448224539</v>
+        <v>3866.806634474071</v>
       </c>
       <c r="Q7">
         <v>1200</v>
@@ -8315,20 +8390,68 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>1650</v>
+      </c>
+      <c r="C8">
+        <v>1027</v>
+      </c>
+      <c r="D8">
+        <v>2123</v>
+      </c>
+      <c r="E8">
+        <v>41107</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>29871</v>
+      </c>
+      <c r="C9">
+        <v>28128</v>
+      </c>
+      <c r="D9">
+        <v>15061</v>
+      </c>
+      <c r="E9">
+        <v>74328</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>25824</v>
+      </c>
+      <c r="C10">
+        <v>11645</v>
+      </c>
+      <c r="D10">
+        <v>15195</v>
+      </c>
+      <c r="E10">
+        <v>127092</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B11">
+        <v>16642</v>
+      </c>
+      <c r="C11">
+        <v>11392</v>
+      </c>
+      <c r="D11">
+        <v>43488</v>
+      </c>
+      <c r="E11">
+        <v>71073</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -8534,7 +8657,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8564,19 +8687,19 @@
       </c>
       <c r="B2" s="5">
         <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
-        <v>16736</v>
+        <v>8392.375</v>
       </c>
       <c r="C2" s="6">
         <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
-        <v>11440.75</v>
+        <v>6557.25</v>
       </c>
       <c r="D2" s="6">
         <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
-        <v>15777.75</v>
+        <v>8573.25</v>
       </c>
       <c r="E2" s="6">
         <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
-        <v>60593.5</v>
+        <v>30558</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8585,19 +8708,19 @@
       </c>
       <c r="B3" s="2">
         <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
-        <v>6194.5154505148075</v>
+        <v>4262.3627289898895</v>
       </c>
       <c r="C3" s="2">
         <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
-        <v>5451.1099080065032</v>
+        <v>3216.3875851977609</v>
       </c>
       <c r="D3" s="2">
         <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
-        <v>8186.1583824465552</v>
+        <v>4706.3661435109052</v>
       </c>
       <c r="E3" s="2">
         <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
-        <v>15747.107324309864</v>
+        <v>13493.071978929462</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -8605,16 +8728,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C4">
-        <v>95</v>
+        <v>6570</v>
       </c>
       <c r="D4">
-        <v>78</v>
+        <v>5337</v>
       </c>
       <c r="E4">
-        <v>31032</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8622,16 +8745,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>28033</v>
+        <v>51</v>
       </c>
       <c r="C5">
-        <v>26326</v>
+        <v>54</v>
       </c>
       <c r="D5">
-        <v>11292</v>
+        <v>52</v>
       </c>
       <c r="E5">
-        <v>49461</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -8639,16 +8762,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>23987</v>
+        <v>51</v>
       </c>
       <c r="C6">
-        <v>9756</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>12951</v>
+        <v>59</v>
       </c>
       <c r="E6">
-        <v>104918</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -8656,36 +8779,84 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>14819</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>9586</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>38790</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>56963</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>105</v>
+      </c>
+      <c r="C8">
+        <v>95</v>
+      </c>
+      <c r="D8">
+        <v>78</v>
+      </c>
+      <c r="E8">
+        <v>31032</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>28033</v>
+      </c>
+      <c r="C9">
+        <v>26326</v>
+      </c>
+      <c r="D9">
+        <v>11292</v>
+      </c>
+      <c r="E9">
+        <v>49461</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>23987</v>
+      </c>
+      <c r="C10">
+        <v>9756</v>
+      </c>
+      <c r="D10">
+        <v>12951</v>
+      </c>
+      <c r="E10">
+        <v>104918</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B11">
+        <v>14819</v>
+      </c>
+      <c r="C11">
+        <v>9586</v>
+      </c>
+      <c r="D11">
+        <v>38790</v>
+      </c>
+      <c r="E11">
+        <v>56963</v>
       </c>
     </row>
   </sheetData>
@@ -8698,7 +8869,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8728,19 +8899,19 @@
       </c>
       <c r="B2" s="5">
         <f>AVERAGE(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))</f>
-        <v>1759.75</v>
+        <v>1408.75</v>
       </c>
       <c r="C2" s="6">
         <f>AVERAGE(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))</f>
-        <v>1605.5</v>
+        <v>1395.25</v>
       </c>
       <c r="D2" s="6">
         <f>AVERAGE(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))</f>
-        <v>3188</v>
+        <v>2333.375</v>
       </c>
       <c r="E2" s="6">
         <f>AVERAGE(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))</f>
-        <v>17805.5</v>
+        <v>12470.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -8749,19 +8920,19 @@
       </c>
       <c r="B3" s="2">
         <f>_xlfn.STDEV.S(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26)))/SQRT(COUNT(B4:INDEX(B4:B26, MATCH(9.99999999999999E+307,B4:B26))))</f>
-        <v>71.998119188397325</v>
+        <v>138.10616387402845</v>
       </c>
       <c r="C3" s="2">
         <f>_xlfn.STDEV.S(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26)))/SQRT(COUNT(C4:INDEX(C4:C26, MATCH(9.99999999999999E+307,C4:C26))))</f>
-        <v>225.75595230248084</v>
+        <v>162.1808679486314</v>
       </c>
       <c r="D3" s="2">
         <f>_xlfn.STDEV.S(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26)))/SQRT(COUNT(D4:INDEX(D4:D26, MATCH(9.99999999999999E+307,D4:D26))))</f>
-        <v>633.45889106292179</v>
+        <v>471.24095055729487</v>
       </c>
       <c r="E3" s="2">
         <f>_xlfn.STDEV.S(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26)))/SQRT(COUNT(E4:INDEX(E4:E26, MATCH(9.99999999999999E+307,E4:E26))))</f>
-        <v>3444.3906209952438</v>
+        <v>2746.1141441784866</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -8769,16 +8940,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1544</v>
+        <v>1058</v>
       </c>
       <c r="C4">
-        <v>931</v>
+        <v>1802</v>
       </c>
       <c r="D4">
-        <v>2044</v>
+        <v>2633</v>
       </c>
       <c r="E4">
-        <v>10074</v>
+        <v>13370</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -8786,16 +8957,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1837</v>
+        <v>1172</v>
       </c>
       <c r="C5">
-        <v>1801</v>
+        <v>985</v>
       </c>
       <c r="D5">
-        <v>3768</v>
+        <v>1105</v>
       </c>
       <c r="E5">
-        <v>24866</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -8803,16 +8974,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1836</v>
+        <v>982</v>
       </c>
       <c r="C6">
-        <v>1888</v>
+        <v>983</v>
       </c>
       <c r="D6">
-        <v>2243</v>
+        <v>1067</v>
       </c>
       <c r="E6">
-        <v>22173</v>
+        <v>4827</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -8820,36 +8991,84 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1822</v>
+        <v>1019</v>
       </c>
       <c r="C7">
-        <v>1802</v>
+        <v>970</v>
       </c>
       <c r="D7">
-        <v>4697</v>
+        <v>1110</v>
       </c>
       <c r="E7">
-        <v>14109</v>
+        <v>4763</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>1544</v>
+      </c>
+      <c r="C8">
+        <v>931</v>
+      </c>
+      <c r="D8">
+        <v>2044</v>
+      </c>
+      <c r="E8">
+        <v>10074</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>1837</v>
+      </c>
+      <c r="C9">
+        <v>1801</v>
+      </c>
+      <c r="D9">
+        <v>3768</v>
+      </c>
+      <c r="E9">
+        <v>24866</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>1836</v>
+      </c>
+      <c r="C10">
+        <v>1888</v>
+      </c>
+      <c r="D10">
+        <v>2243</v>
+      </c>
+      <c r="E10">
+        <v>22173</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1822</v>
+      </c>
+      <c r="C11">
+        <v>1802</v>
+      </c>
+      <c r="D11">
+        <v>4697</v>
+      </c>
+      <c r="E11">
+        <v>14109</v>
       </c>
     </row>
   </sheetData>
@@ -8861,8 +9080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" zoomScalePageLayoutView="171" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A51" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Iterating as paper diagrams
</commit_message>
<xml_diff>
--- a/Swift_Experiments/strategy_1/analysis/strategy_1_analysis_cleaned.xlsx
+++ b/Swift_Experiments/strategy_1/analysis/strategy_1_analysis_cleaned.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -33,7 +33,7 @@
     <definedName name="Tw_Submitting_task_stampede_gordon" localSheetId="4">Tw_stampede_gordon!$B$4:$E$11</definedName>
     <definedName name="Tw_Submitting_task_stampede_gordon_1" localSheetId="4">Tw_stampede_gordon!$B$4:$E$11</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -343,26 +343,44 @@
             <a:pPr>
               <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1"/>
-              <a:t>Time to Completion (TTC) - Swift</a:t>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
+              <a:t>Experiment 1 - TTC - Swift</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
               <a:t> on </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
               <a:t>Stampede and Gordon</a:t>
             </a:r>
           </a:p>
@@ -384,14 +402,11 @@
           <a:pPr>
             <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -599,11 +614,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131090944"/>
-        <c:axId val="-2130778992"/>
+        <c:axId val="-2114549264"/>
+        <c:axId val="-2114605904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131090944"/>
+        <c:axId val="-2114549264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,18 +633,22 @@
                 <a:pPr>
                   <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t>Number of Tasks</a:t>
                 </a:r>
               </a:p>
@@ -651,14 +670,11 @@
               <a:pPr>
                 <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -689,20 +705,17 @@
             <a:pPr>
               <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130778992"/>
+        <c:crossAx val="-2114605904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -710,7 +723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130778992"/>
+        <c:axId val="-2114605904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000.0"/>
@@ -740,25 +753,43 @@
                 <a:pPr>
                   <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t>Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t> (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="2000"/>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -778,14 +809,11 @@
               <a:pPr>
                 <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -810,20 +838,17 @@
             <a:pPr>
               <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131090944"/>
+        <c:crossAx val="-2114549264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2000.0"/>
@@ -854,14 +879,11 @@
           <a:pPr>
             <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -923,29 +945,76 @@
             <a:pPr>
               <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1"/>
-              <a:t>Waiting Time (Tw) - Swift</a:t>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
+              <a:t>Experiment 1</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
+              <a:t> -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
+              <a:t> Tw - Swift</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
               <a:t> on </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:rPr lang="en-US" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
+              </a:rPr>
               <a:t>Stampede and Gordon</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="2000"/>
+            <a:endParaRPr lang="en-US" sz="2000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -965,14 +1034,11 @@
           <a:pPr>
             <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1127,11 +1193,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132113168"/>
-        <c:axId val="-2132107264"/>
+        <c:axId val="2142272416"/>
+        <c:axId val="-2114632528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132113168"/>
+        <c:axId val="2142272416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,18 +1212,22 @@
                 <a:pPr>
                   <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t>Number of Tasks</a:t>
                 </a:r>
               </a:p>
@@ -1179,14 +1249,11 @@
               <a:pPr>
                 <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1217,20 +1284,17 @@
             <a:pPr>
               <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132107264"/>
+        <c:crossAx val="-2114632528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132107264"/>
+        <c:axId val="-2114632528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000.0"/>
@@ -1268,25 +1332,43 @@
                 <a:pPr>
                   <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t>Time</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                    <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                    <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                  </a:rPr>
                   <a:t> (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="2000"/>
+                <a:endParaRPr lang="en-US" sz="2000">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1306,14 +1388,11 @@
               <a:pPr>
                 <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                  <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                  <a:cs typeface="NimbusRomNo9L" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1338,20 +1417,17 @@
             <a:pPr>
               <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="NimbusRomNo9L" charset="0"/>
+                <a:ea typeface="NimbusRomNo9L" charset="0"/>
+                <a:cs typeface="NimbusRomNo9L" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132113168"/>
+        <c:crossAx val="2142272416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1381,14 +1457,11 @@
           <a:pPr>
             <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="NimbusRomNo9L" charset="0"/>
+              <a:ea typeface="NimbusRomNo9L" charset="0"/>
+              <a:cs typeface="NimbusRomNo9L" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1677,11 +1750,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132071712"/>
-        <c:axId val="-2132065808"/>
+        <c:axId val="-2122489488"/>
+        <c:axId val="-2122507792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132071712"/>
+        <c:axId val="-2122489488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1853,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132065808"/>
+        <c:crossAx val="-2122507792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1788,7 +1861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132065808"/>
+        <c:axId val="-2122507792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60000.0"/>
@@ -1901,7 +1974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132071712"/>
+        <c:crossAx val="-2122489488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2096,7 +2169,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2291,11 +2363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133487344"/>
-        <c:axId val="-2133474624"/>
+        <c:axId val="-2117777504"/>
+        <c:axId val="-2117774976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133487344"/>
+        <c:axId val="-2117777504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2327,7 +2399,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2394,7 +2465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133474624"/>
+        <c:crossAx val="-2117774976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2402,7 +2473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133474624"/>
+        <c:axId val="-2117774976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -2454,7 +2525,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2515,7 +2585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133487344"/>
+        <c:crossAx val="-2117777504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2727,7 +2797,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2919,11 +2988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132023168"/>
-        <c:axId val="-2132017264"/>
+        <c:axId val="-2118113680"/>
+        <c:axId val="-2114618208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132023168"/>
+        <c:axId val="-2118113680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2955,7 +3024,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3022,7 +3090,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132017264"/>
+        <c:crossAx val="-2114618208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3030,7 +3098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132017264"/>
+        <c:axId val="-2114618208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -3082,7 +3150,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3143,7 +3210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132023168"/>
+        <c:crossAx val="-2118113680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3543,11 +3610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131980048"/>
-        <c:axId val="-2131974144"/>
+        <c:axId val="-2114526576"/>
+        <c:axId val="-2114496608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131980048"/>
+        <c:axId val="-2114526576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3645,7 +3712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131974144"/>
+        <c:crossAx val="-2114496608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3653,7 +3720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131974144"/>
+        <c:axId val="-2114496608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12000.0"/>
@@ -3765,7 +3832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131980048"/>
+        <c:crossAx val="-2114526576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7279,7 +7346,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7291,7 +7358,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7299,7 +7366,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TTC-Time_to_completion-stampede_gordon_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7311,7 +7378,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Te-Executing_task-stampede_gordon" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>